<commit_message>
Code/files added for the data management guidline document.
</commit_message>
<xml_diff>
--- a/ALL_DATA/TIFF_seagrass/2018_data_efforts/cages.xlsx
+++ b/ALL_DATA/TIFF_seagrass/2018_data_efforts/cages.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiff/Desktop/R Studio/APECS-master-repos/ALL_DATA/TIFF_seagrass/2018_data_efforts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3B180C-290E-964B-9523-AE8993C74D68}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D7C3F6-9135-1D45-9B74-9FF67E8259F5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="120" windowWidth="27640" windowHeight="16940" xr2:uid="{6CC17970-CAB1-0C4A-A9BC-FC82B0E49AD1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="worked" sheetId="1" r:id="rId1"/>
+    <sheet name="raw" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -170,7 +171,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -205,8 +206,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +525,7 @@
   <dimension ref="A1:AT61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AU16" sqref="AU16"/>
+      <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="AK2">
-        <f t="shared" ref="AJ2:AL2" si="0">SUM(AG2:AG7)</f>
+        <f t="shared" ref="AK2" si="0">SUM(AG2:AG7)</f>
         <v>0</v>
       </c>
       <c r="AL2">
@@ -1291,7 +1292,7 @@
         <v>0.71666666666666667</v>
       </c>
       <c r="AT7">
-        <f t="shared" ref="AS7:AT7" si="1">AVERAGE(AL2:AL61)</f>
+        <f t="shared" ref="AT7" si="1">AVERAGE(AL2:AL61)</f>
         <v>2.0000000000000004</v>
       </c>
     </row>
@@ -1405,7 +1406,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="AK8">
-        <f t="shared" ref="AJ8:AL8" si="2">SUM(AG8:AG13)</f>
+        <f t="shared" ref="AK8" si="2">SUM(AG8:AG13)</f>
         <v>0</v>
       </c>
       <c r="AL8">
@@ -2029,7 +2030,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AK14">
-        <f t="shared" ref="AJ14:AL14" si="3">SUM(AG14:AG19)</f>
+        <f t="shared" ref="AK14" si="3">SUM(AG14:AG19)</f>
         <v>2</v>
       </c>
       <c r="AL14">
@@ -2637,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="AK20">
-        <f t="shared" ref="AJ20:AL20" si="4">SUM(AG20:AG25)</f>
+        <f t="shared" ref="AK20" si="4">SUM(AG20:AG25)</f>
         <v>1</v>
       </c>
       <c r="AL20">
@@ -3265,7 +3266,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="AK26">
-        <f t="shared" ref="AJ26:AL26" si="5">SUM(AG26:AG31)</f>
+        <f t="shared" ref="AK26" si="5">SUM(AG26:AG31)</f>
         <v>0</v>
       </c>
       <c r="AL26">
@@ -3893,7 +3894,7 @@
         <v>2.5</v>
       </c>
       <c r="AK32">
-        <f t="shared" ref="AJ32:AL32" si="6">SUM(AG32:AG37)</f>
+        <f t="shared" ref="AK32" si="6">SUM(AG32:AG37)</f>
         <v>1</v>
       </c>
       <c r="AL32">
@@ -4521,7 +4522,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="AK38">
-        <f t="shared" ref="AJ38:AL38" si="7">SUM(AG38:AG43)</f>
+        <f t="shared" ref="AK38" si="7">SUM(AG38:AG43)</f>
         <v>0</v>
       </c>
       <c r="AL38">
@@ -5149,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="AK44">
-        <f t="shared" ref="AJ44:AL44" si="8">SUM(AG44:AG49)</f>
+        <f t="shared" ref="AK44" si="8">SUM(AG44:AG49)</f>
         <v>0</v>
       </c>
       <c r="AL44">
@@ -5777,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="AK50">
-        <f t="shared" ref="AJ50:AL50" si="9">SUM(AG50:AG55)</f>
+        <f t="shared" ref="AK50" si="9">SUM(AG50:AG55)</f>
         <v>6</v>
       </c>
       <c r="AL50">
@@ -6405,7 +6406,7 @@
         <v>0.5</v>
       </c>
       <c r="AK56">
-        <f t="shared" ref="AJ56:AL56" si="10">SUM(AG56:AG61)</f>
+        <f t="shared" ref="AK56" si="10">SUM(AG56:AG61)</f>
         <v>1</v>
       </c>
       <c r="AL56">
@@ -6926,4 +6927,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9CB7F4-ACFE-274A-93F0-84498A7E1979}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>